<commit_message>
update lernjournal 4 - change times
</commit_message>
<xml_diff>
--- a/Documentation/ProjectOrganisation/team1_aufgabe4_lernjournal.xlsx
+++ b/Documentation/ProjectOrganisation/team1_aufgabe4_lernjournal.xlsx
@@ -1,32 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marku\eclipse-workspace\swiss-qr-code\Documentation\ProjectOrganisation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolas/eclipse-workspace/swiss-qr-code/Documentation/ProjectOrganisation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B800A9-F378-491C-B775-B9CF756D5A57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A375A08C-2682-8249-9860-498E7B4B3CEE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28840" windowHeight="17480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lernjournal" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -563,20 +552,21 @@
   <dimension ref="A1:IW59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="90.8984375" style="2" customWidth="1"/>
-    <col min="2" max="3" width="8.5" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10.69921875" style="3" customWidth="1"/>
-    <col min="5" max="17" width="10.69921875" style="2" customWidth="1"/>
-    <col min="18" max="257" width="10.69921875" style="4" customWidth="1"/>
-    <col min="258" max="1024" width="10.69921875" customWidth="1"/>
+    <col min="1" max="1" width="90.83203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="13" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="3" customWidth="1"/>
+    <col min="5" max="17" width="10.6640625" style="2" customWidth="1"/>
+    <col min="18" max="257" width="10.6640625" style="4" customWidth="1"/>
+    <col min="258" max="1024" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -597,7 +587,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" s="4" customFormat="1" ht="82.8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -618,7 +608,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -637,7 +627,7 @@
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
     </row>
-    <row r="4" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -656,7 +646,7 @@
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
     </row>
-    <row r="5" spans="1:17" s="4" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
         <v>14</v>
       </c>
@@ -677,7 +667,7 @@
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
     </row>
-    <row r="6" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -696,7 +686,7 @@
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
     </row>
-    <row r="7" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -715,7 +705,7 @@
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
     </row>
-    <row r="8" spans="1:17" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
@@ -738,7 +728,7 @@
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
     </row>
-    <row r="9" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -757,7 +747,7 @@
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
     </row>
-    <row r="10" spans="1:17" s="4" customFormat="1" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" s="4" customFormat="1" ht="28.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="6" t="s">
         <v>3</v>
       </c>
@@ -784,19 +774,19 @@
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
     </row>
-    <row r="11" spans="1:17" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B11" s="9">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="C11" s="10">
         <f>B11/60</f>
-        <v>2.5</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="D11" s="11">
-        <v>44157</v>
+        <v>44156</v>
       </c>
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
@@ -812,16 +802,16 @@
       <c r="P11" s="12"/>
       <c r="Q11" s="12"/>
     </row>
-    <row r="12" spans="1:17" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" s="9">
-        <v>30</v>
+        <v>150</v>
       </c>
       <c r="C12" s="10">
         <f>B12/60</f>
-        <v>0.5</v>
+        <v>2.5</v>
       </c>
       <c r="D12" s="11">
         <v>44157</v>
@@ -840,19 +830,19 @@
       <c r="P12" s="12"/>
       <c r="Q12" s="12"/>
     </row>
-    <row r="13" spans="1:17" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13" s="9">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="C13" s="10">
         <f>B13/60</f>
-        <v>0.83333333333333337</v>
+        <v>0.5</v>
       </c>
       <c r="D13" s="11">
-        <v>44156</v>
+        <v>44157</v>
       </c>
       <c r="E13" s="12"/>
       <c r="F13" s="12"/>
@@ -863,12 +853,8 @@
       <c r="K13" s="12"/>
       <c r="L13" s="12"/>
       <c r="M13" s="12"/>
-      <c r="N13" s="12"/>
-      <c r="O13" s="12"/>
-      <c r="P13" s="12"/>
-      <c r="Q13" s="12"/>
-    </row>
-    <row r="14" spans="1:17" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:17" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
       <c r="C14" s="10">
@@ -890,7 +876,7 @@
       <c r="P14" s="12"/>
       <c r="Q14" s="12"/>
     </row>
-    <row r="15" spans="1:17" s="13" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" s="13" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="12"/>
       <c r="B15" s="12"/>
       <c r="C15" s="12"/>
@@ -909,7 +895,7 @@
       <c r="P15" s="12"/>
       <c r="Q15" s="12"/>
     </row>
-    <row r="16" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.15">
       <c r="A16" s="15" t="s">
         <v>7</v>
       </c>
@@ -936,7 +922,7 @@
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
     </row>
-    <row r="17" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -955,7 +941,7 @@
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
     </row>
-    <row r="18" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -974,7 +960,7 @@
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
     </row>
-    <row r="19" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -993,7 +979,7 @@
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
     </row>
-    <row r="20" spans="1:17" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A20" s="5" t="s">
         <v>9</v>
       </c>
@@ -1016,7 +1002,7 @@
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
     </row>
-    <row r="21" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -1035,7 +1021,7 @@
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
     </row>
-    <row r="22" spans="1:17" s="4" customFormat="1" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" s="4" customFormat="1" ht="28.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="6" t="s">
         <v>3</v>
       </c>
@@ -1062,19 +1048,19 @@
       <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
     </row>
-    <row r="23" spans="1:17" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B23" s="9">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="C23" s="10">
         <f>B23/60</f>
-        <v>2.5</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="D23" s="11">
-        <v>44126</v>
+        <v>44156</v>
       </c>
       <c r="E23" s="12"/>
       <c r="F23" s="12"/>
@@ -1090,19 +1076,19 @@
       <c r="P23" s="12"/>
       <c r="Q23" s="12"/>
     </row>
-    <row r="24" spans="1:17" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B24" s="9">
-        <v>30</v>
+        <v>150</v>
       </c>
       <c r="C24" s="10">
         <f>B24/60</f>
-        <v>0.5</v>
+        <v>2.5</v>
       </c>
       <c r="D24" s="11">
-        <v>44126</v>
+        <v>44157</v>
       </c>
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
@@ -1112,25 +1098,20 @@
       <c r="J24" s="12"/>
       <c r="K24" s="12"/>
       <c r="L24" s="12"/>
-      <c r="M24" s="12"/>
-      <c r="N24" s="12"/>
-      <c r="O24" s="12"/>
-      <c r="P24" s="12"/>
-      <c r="Q24" s="12"/>
-    </row>
-    <row r="25" spans="1:17" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:17" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B25" s="9">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="C25" s="10">
         <f>B25/60</f>
-        <v>0.83333333333333337</v>
+        <v>0.5</v>
       </c>
       <c r="D25" s="11">
-        <v>44156</v>
+        <v>44157</v>
       </c>
       <c r="E25" s="12"/>
       <c r="F25" s="12"/>
@@ -1140,13 +1121,8 @@
       <c r="J25" s="12"/>
       <c r="K25" s="12"/>
       <c r="L25" s="12"/>
-      <c r="M25" s="12"/>
-      <c r="N25" s="12"/>
-      <c r="O25" s="12"/>
-      <c r="P25" s="12"/>
-      <c r="Q25" s="12"/>
-    </row>
-    <row r="26" spans="1:17" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:17" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="9"/>
       <c r="B26" s="9"/>
       <c r="C26" s="10">
@@ -1162,13 +1138,8 @@
       <c r="J26" s="12"/>
       <c r="K26" s="12"/>
       <c r="L26" s="12"/>
-      <c r="M26" s="12"/>
-      <c r="N26" s="12"/>
-      <c r="O26" s="12"/>
-      <c r="P26" s="12"/>
-      <c r="Q26" s="12"/>
-    </row>
-    <row r="27" spans="1:17" s="13" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:17" s="13" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="12"/>
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
@@ -1181,13 +1152,8 @@
       <c r="J27" s="12"/>
       <c r="K27" s="12"/>
       <c r="L27" s="12"/>
-      <c r="M27" s="12"/>
-      <c r="N27" s="12"/>
-      <c r="O27" s="12"/>
-      <c r="P27" s="12"/>
-      <c r="Q27" s="12"/>
-    </row>
-    <row r="28" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:17" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.15">
       <c r="A28" s="15" t="s">
         <v>7</v>
       </c>
@@ -1208,13 +1174,8 @@
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
-      <c r="M28" s="2"/>
-      <c r="N28" s="2"/>
-      <c r="O28" s="2"/>
-      <c r="P28" s="2"/>
-      <c r="Q28" s="2"/>
-    </row>
-    <row r="29" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -1227,13 +1188,8 @@
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
-      <c r="M29" s="2"/>
-      <c r="N29" s="2"/>
-      <c r="O29" s="2"/>
-      <c r="P29" s="2"/>
-      <c r="Q29" s="2"/>
-    </row>
-    <row r="30" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -1246,13 +1202,8 @@
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
-      <c r="M30" s="2"/>
-      <c r="N30" s="2"/>
-      <c r="O30" s="2"/>
-      <c r="P30" s="2"/>
-      <c r="Q30" s="2"/>
-    </row>
-    <row r="31" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -1265,13 +1216,8 @@
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
-      <c r="M31" s="2"/>
-      <c r="N31" s="2"/>
-      <c r="O31" s="2"/>
-      <c r="P31" s="2"/>
-      <c r="Q31" s="2"/>
-    </row>
-    <row r="32" spans="1:17" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:17" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A32" s="5" t="s">
         <v>10</v>
       </c>
@@ -1288,13 +1234,8 @@
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
-      <c r="M32" s="2"/>
-      <c r="N32" s="2"/>
-      <c r="O32" s="2"/>
-      <c r="P32" s="2"/>
-      <c r="Q32" s="2"/>
-    </row>
-    <row r="33" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -1307,13 +1248,8 @@
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
-      <c r="M33" s="2"/>
-      <c r="N33" s="2"/>
-      <c r="O33" s="2"/>
-      <c r="P33" s="2"/>
-      <c r="Q33" s="2"/>
-    </row>
-    <row r="34" spans="1:17" s="4" customFormat="1" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:17" s="4" customFormat="1" ht="28.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="6" t="s">
         <v>3</v>
       </c>
@@ -1334,25 +1270,20 @@
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
-      <c r="M34" s="2"/>
-      <c r="N34" s="2"/>
-      <c r="O34" s="2"/>
-      <c r="P34" s="2"/>
-      <c r="Q34" s="2"/>
-    </row>
-    <row r="35" spans="1:17" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:17" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B35" s="9">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="C35" s="10">
         <f>B35/60</f>
-        <v>2.5</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="D35" s="11">
-        <v>44126</v>
+        <v>44156</v>
       </c>
       <c r="E35" s="12"/>
       <c r="F35" s="12"/>
@@ -1362,25 +1293,20 @@
       <c r="J35" s="12"/>
       <c r="K35" s="12"/>
       <c r="L35" s="12"/>
-      <c r="M35" s="12"/>
-      <c r="N35" s="12"/>
-      <c r="O35" s="12"/>
-      <c r="P35" s="12"/>
-      <c r="Q35" s="12"/>
-    </row>
-    <row r="36" spans="1:17" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:17" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B36" s="9">
-        <v>30</v>
+        <v>150</v>
       </c>
       <c r="C36" s="10">
         <f>B36/60</f>
-        <v>0.5</v>
+        <v>2.5</v>
       </c>
       <c r="D36" s="11">
-        <v>44126</v>
+        <v>44157</v>
       </c>
       <c r="E36" s="12"/>
       <c r="F36" s="12"/>
@@ -1390,25 +1316,20 @@
       <c r="J36" s="12"/>
       <c r="K36" s="12"/>
       <c r="L36" s="12"/>
-      <c r="M36" s="12"/>
-      <c r="N36" s="12"/>
-      <c r="O36" s="12"/>
-      <c r="P36" s="12"/>
-      <c r="Q36" s="12"/>
-    </row>
-    <row r="37" spans="1:17" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:17" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B37" s="9">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="C37" s="10">
         <f>B37/60</f>
-        <v>0.83333333333333337</v>
+        <v>0.5</v>
       </c>
       <c r="D37" s="11">
-        <v>44156</v>
+        <v>44157</v>
       </c>
       <c r="E37" s="12"/>
       <c r="F37" s="12"/>
@@ -1418,13 +1339,8 @@
       <c r="J37" s="12"/>
       <c r="K37" s="12"/>
       <c r="L37" s="12"/>
-      <c r="M37" s="12"/>
-      <c r="N37" s="12"/>
-      <c r="O37" s="12"/>
-      <c r="P37" s="12"/>
-      <c r="Q37" s="12"/>
-    </row>
-    <row r="38" spans="1:17" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:17" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="9"/>
       <c r="B38" s="9"/>
       <c r="C38" s="10">
@@ -1440,13 +1356,8 @@
       <c r="J38" s="12"/>
       <c r="K38" s="12"/>
       <c r="L38" s="12"/>
-      <c r="M38" s="12"/>
-      <c r="N38" s="12"/>
-      <c r="O38" s="12"/>
-      <c r="P38" s="12"/>
-      <c r="Q38" s="12"/>
-    </row>
-    <row r="39" spans="1:17" s="13" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:17" s="13" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="12"/>
       <c r="B39" s="12"/>
       <c r="C39" s="12"/>
@@ -1465,7 +1376,7 @@
       <c r="P39" s="12"/>
       <c r="Q39" s="12"/>
     </row>
-    <row r="40" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.15">
       <c r="A40" s="15" t="s">
         <v>7</v>
       </c>
@@ -1492,7 +1403,7 @@
       <c r="P40" s="2"/>
       <c r="Q40" s="2"/>
     </row>
-    <row r="41" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -1511,7 +1422,7 @@
       <c r="P41" s="2"/>
       <c r="Q41" s="2"/>
     </row>
-    <row r="42" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -1530,7 +1441,7 @@
       <c r="P42" s="2"/>
       <c r="Q42" s="2"/>
     </row>
-    <row r="43" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -1549,7 +1460,7 @@
       <c r="P43" s="2"/>
       <c r="Q43" s="2"/>
     </row>
-    <row r="44" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -1568,7 +1479,7 @@
       <c r="P44" s="2"/>
       <c r="Q44" s="2"/>
     </row>
-    <row r="45" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -1587,7 +1498,7 @@
       <c r="P45" s="2"/>
       <c r="Q45" s="2"/>
     </row>
-    <row r="46" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -1606,7 +1517,7 @@
       <c r="P46" s="2"/>
       <c r="Q46" s="2"/>
     </row>
-    <row r="47" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -1625,7 +1536,7 @@
       <c r="P47" s="2"/>
       <c r="Q47" s="2"/>
     </row>
-    <row r="48" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -1644,7 +1555,7 @@
       <c r="P48" s="2"/>
       <c r="Q48" s="2"/>
     </row>
-    <row r="49" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -1663,7 +1574,7 @@
       <c r="P49" s="2"/>
       <c r="Q49" s="2"/>
     </row>
-    <row r="50" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -1682,7 +1593,7 @@
       <c r="P50" s="2"/>
       <c r="Q50" s="2"/>
     </row>
-    <row r="51" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -1701,7 +1612,7 @@
       <c r="P51" s="2"/>
       <c r="Q51" s="2"/>
     </row>
-    <row r="52" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -1720,7 +1631,7 @@
       <c r="P52" s="2"/>
       <c r="Q52" s="2"/>
     </row>
-    <row r="53" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -1739,7 +1650,7 @@
       <c r="P53" s="2"/>
       <c r="Q53" s="2"/>
     </row>
-    <row r="54" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -1758,7 +1669,7 @@
       <c r="P54" s="2"/>
       <c r="Q54" s="2"/>
     </row>
-    <row r="55" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -1777,7 +1688,7 @@
       <c r="P55" s="2"/>
       <c r="Q55" s="2"/>
     </row>
-    <row r="56" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -1796,7 +1707,7 @@
       <c r="P56" s="2"/>
       <c r="Q56" s="2"/>
     </row>
-    <row r="57" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -1815,7 +1726,7 @@
       <c r="P57" s="2"/>
       <c r="Q57" s="2"/>
     </row>
-    <row r="58" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -1834,7 +1745,7 @@
       <c r="P58" s="2"/>
       <c r="Q58" s="2"/>
     </row>
-    <row r="59" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>

</xml_diff>